<commit_message>
Bhavin - Error Solve
</commit_message>
<xml_diff>
--- a/AccountManegments.Web/wwwroot/UploadExcelFile/ItemMasterDetails.xlsx
+++ b/AccountManegments.Web/wwwroot/UploadExcelFile/ItemMasterDetails.xlsx
@@ -1,32 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonuf\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40178AD7-69B7-401F-89CD-2645A8E2199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FC0A07-C221-4E90-9F45-51897A41C34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserAttendanceModel" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
-  <si>
-    <t>CreatedOn</t>
-  </si>
-  <si>
-    <t>ItemId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ItemName</t>
   </si>
@@ -37,9 +32,6 @@
     <t>PricePerUnit</t>
   </si>
   <si>
-    <t>IsWithGst</t>
-  </si>
-  <si>
     <t>GSTAmount</t>
   </si>
   <si>
@@ -49,34 +41,10 @@
     <t>HSNCode</t>
   </si>
   <si>
-    <t>IsApproved</t>
-  </si>
-  <si>
-    <t>IsDeleted</t>
-  </si>
-  <si>
-    <t>CreatedBy</t>
-  </si>
-  <si>
-    <t>UpdatedBy</t>
-  </si>
-  <si>
-    <t>UpdatedOn</t>
-  </si>
-  <si>
-    <t>Apple Iphone 15(128GB,Blue)</t>
-  </si>
-  <si>
-    <t>27192320-4006-4822-A498-EAC8D061667F</t>
-  </si>
-  <si>
-    <t>P553BB94-4869-4A98-9612-8FD81E37CA5B</t>
-  </si>
-  <si>
-    <t>fd338bac-80e4-419a-a490-4035ce234603</t>
-  </si>
-  <si>
-    <t>Combo kit of  Colours</t>
+    <t>Washing Machine</t>
+  </si>
+  <si>
+    <t>Valves</t>
   </si>
 </sst>
 </file>
@@ -111,9 +79,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,23 +99,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N3" totalsRowShown="0">
-  <autoFilter ref="A1:N3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ItemId"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F3" totalsRowShown="0">
+  <autoFilter ref="A1:F3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ItemName"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="UnitType"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PricePerUnit"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IsWithGst"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="GSTAmount"/>
     <tableColumn id="7" xr3:uid="{239E600E-326F-4FE2-9FC7-2F01A3A9CF29}" name="GSTPer"/>
     <tableColumn id="8" xr3:uid="{D2286FF1-1391-4B45-B297-C265B41E7C30}" name="HSNCode"/>
-    <tableColumn id="9" xr3:uid="{FF3123E7-C6DE-471C-AC1D-DDC5CF5580E8}" name="IsApproved"/>
-    <tableColumn id="10" xr3:uid="{AD179543-B0AD-4225-895A-9FDEC34DF764}" name="IsDeleted"/>
-    <tableColumn id="11" xr3:uid="{C39E47AC-A50E-4091-A523-173ABD47C631}" name="CreatedBy"/>
-    <tableColumn id="12" xr3:uid="{39480412-658F-43CA-887B-56D1A9CE07AE}" name="CreatedOn"/>
-    <tableColumn id="13" xr3:uid="{7EC4FA59-D34E-4466-810D-20DB67F239BE}" name="UpdatedBy"/>
-    <tableColumn id="14" xr3:uid="{1DE29B32-2823-4064-8B8C-972715A01E26}" name="UpdatedOn"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -439,166 +398,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="36.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="35" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>79900</v>
+      </c>
+      <c r="D2">
+        <v>3995</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>85171300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>79900</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3995</v>
-      </c>
-      <c r="G2">
-        <v>0.2</v>
-      </c>
-      <c r="H2">
-        <v>85171300</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1">
-        <v>45373.633487615742</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="1">
-        <v>45373.631048229166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>2550</v>
       </c>
       <c r="D3">
-        <v>2550</v>
+        <v>625</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F3">
-        <v>625</v>
-      </c>
-      <c r="G3">
-        <v>0.3</v>
-      </c>
-      <c r="H3">
         <v>45123</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1">
-        <v>45373.633487615742</v>
-      </c>
-      <c r="M3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="1">
-        <v>45373.633487615742</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53978F4-DB24-486A-8C2D-A9331AD606D6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>